<commit_message>
Ranking atualizado trivia outubro
</commit_message>
<xml_diff>
--- a/assets/data/ranking_anual.xlsx
+++ b/assets/data/ranking_anual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bih14\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD46D4E-2DE6-40A5-905D-1214A5AEF883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2EC6465-C114-4273-9D63-E995A86EF162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{17B7C58C-9BD1-4121-BFEB-3B3EBBA28367}"/>
   </bookViews>
@@ -615,7 +615,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -669,8 +669,8 @@
         <v>2</v>
       </c>
       <c r="B2" s="6">
-        <f>SUM(C2:I2)</f>
-        <v>70</v>
+        <f>SUM(C2:J2)</f>
+        <v>85</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -702,7 +702,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="6">
-        <f t="shared" ref="B3:B13" si="0">SUM(C3:I3)</f>
+        <f t="shared" ref="B3:B14" si="0">SUM(C3:J3)</f>
         <v>49</v>
       </c>
       <c r="C3" s="3">
@@ -736,7 +736,7 @@
       </c>
       <c r="B4" s="6">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3">
         <v>10</v>
@@ -769,7 +769,7 @@
       </c>
       <c r="B5" s="6">
         <f t="shared" si="0"/>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C5" s="3">
         <v>2</v>
@@ -802,7 +802,7 @@
       </c>
       <c r="B6" s="6">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -868,7 +868,7 @@
       </c>
       <c r="B8" s="6">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3">
         <v>1</v>
@@ -1065,8 +1065,8 @@
         <v>22</v>
       </c>
       <c r="B14" s="6">
-        <f t="shared" ref="B14" si="1">SUM(C14:I14)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="C14" s="3">
         <v>0</v>

</xml_diff>